<commit_message>
240213 1634 Mac -> Acertado o DELETE e a exportação do Excel para a pasta DOWNLOADS.
</commit_message>
<xml_diff>
--- a/ArquivosExcel/alunos.xlsx
+++ b/ArquivosExcel/alunos.xlsx
@@ -59,15 +59,6 @@
   </x:si>
   <x:si>
     <x:t>leticia@teste.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>teste</x:t>
-  </x:si>
-  <x:si>
-    <x:t>teste@teste.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TURMA C</x:t>
   </x:si>
   <x:si>
     <x:t>Pingo</x:t>
@@ -424,7 +415,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D7"/>
+  <x:dimension ref="A1:D6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -508,23 +499,9 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C6" s="0">
-        <x:v>50</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="A7" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>

</xml_diff>